<commit_message>
Nouveau design du site
</commit_message>
<xml_diff>
--- a/doc/dico_donnees.xlsx
+++ b/doc/dico_donnees.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Nom de la donnée</t>
   </si>
@@ -66,13 +66,28 @@
     <t>tel_membre</t>
   </si>
   <si>
-    <t>numérique</t>
-  </si>
-  <si>
     <t>Pas de chiffre</t>
   </si>
   <si>
     <t>mot_passe_membre</t>
+  </si>
+  <si>
+    <t>id_membre</t>
+  </si>
+  <si>
+    <t>adresse_membre</t>
+  </si>
+  <si>
+    <t>cp_membre</t>
+  </si>
+  <si>
+    <t>ville_membre</t>
+  </si>
+  <si>
+    <t>Numérique</t>
+  </si>
+  <si>
+    <t>Auto incrémenté</t>
   </si>
 </sst>
 </file>
@@ -155,26 +170,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -492,136 +519,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="11">
+        <v>100</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C4" s="2">
         <v>100</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="2">
         <v>100</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2">
+        <v>100</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>100</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2">
+        <v>100</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3">
-        <v>100</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="C11" s="2">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Amélioration du formulaire de contact et envoi du mail
</commit_message>
<xml_diff>
--- a/doc/dico_donnees.xlsx
+++ b/doc/dico_donnees.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>Nom de la donnée</t>
   </si>
@@ -88,6 +88,30 @@
   </si>
   <si>
     <t>Auto incrémenté</t>
+  </si>
+  <si>
+    <t>id_message</t>
+  </si>
+  <si>
+    <t>nom_expediateur_message</t>
+  </si>
+  <si>
+    <t>prenom_expediteur_ message</t>
+  </si>
+  <si>
+    <t>email_expediteur_message</t>
+  </si>
+  <si>
+    <t>corps_message</t>
+  </si>
+  <si>
+    <t>Peut être vide</t>
+  </si>
+  <si>
+    <t>Peut-être vide</t>
+  </si>
+  <si>
+    <t>Champ obligatoire</t>
   </si>
 </sst>
 </file>
@@ -170,12 +194,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -191,18 +227,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,77 +529,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.09765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="4"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="6">
         <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="10"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -723,6 +748,124 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2">
+        <v>100</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
+        <v>255</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2">
+        <v>255</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2">
+        <v>255</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2">
+        <v>255</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Formulaire création d'un article
</commit_message>
<xml_diff>
--- a/doc/dico_donnees.xlsx
+++ b/doc/dico_donnees.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
   <si>
     <t>Nom de la donnée</t>
   </si>
@@ -112,6 +112,33 @@
   </si>
   <si>
     <t>Champ obligatoire</t>
+  </si>
+  <si>
+    <t>id_membre_message</t>
+  </si>
+  <si>
+    <t>id_lettre</t>
+  </si>
+  <si>
+    <t>email_lettre_membre</t>
+  </si>
+  <si>
+    <t>id_article</t>
+  </si>
+  <si>
+    <t>corps_article</t>
+  </si>
+  <si>
+    <t>photo_article</t>
+  </si>
+  <si>
+    <t>date_article</t>
+  </si>
+  <si>
+    <t>auteur_article</t>
+  </si>
+  <si>
+    <t>titre_article</t>
   </si>
 </sst>
 </file>
@@ -212,6 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -227,7 +255,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -544,42 +571,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="8"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -750,7 +777,7 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -770,7 +797,7 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -790,7 +817,7 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -808,7 +835,7 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -828,7 +855,7 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -848,8 +875,8 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>18</v>
+      <c r="A17" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>22</v>
@@ -866,6 +893,140 @@
         <v>29</v>
       </c>
       <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="7">
+        <v>255</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="7">
+        <v>255</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="2">
+        <v>255</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2">
+        <v>255</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2">
+        <v>255</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="2">
+        <v>255</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2">
+        <v>255</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="2">
+        <v>255</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Amélioration de l'inscription à la newsletter
</commit_message>
<xml_diff>
--- a/doc/dico_donnees.xlsx
+++ b/doc/dico_donnees.xlsx
@@ -117,12 +117,6 @@
     <t>id_membre_message</t>
   </si>
   <si>
-    <t>id_lettre</t>
-  </si>
-  <si>
-    <t>email_lettre_membre</t>
-  </si>
-  <si>
     <t>id_article</t>
   </si>
   <si>
@@ -139,6 +133,12 @@
   </si>
   <si>
     <t>titre_article</t>
+  </si>
+  <si>
+    <t>id_abonne</t>
+  </si>
+  <si>
+    <t>email_abonne_membre</t>
   </si>
 </sst>
 </file>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -896,7 +896,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>22</v>
@@ -914,7 +914,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>7</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>22</v>
@@ -948,7 +948,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>11</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>11</v>
@@ -980,7 +980,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
@@ -996,7 +996,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>7</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>11</v>

</xml_diff>